<commit_message>
Actualizacion Scripts: Añadido de tabla LGA_AUTORIZACION
</commit_message>
<xml_diff>
--- a/01-carga-excel/sqlite/docs/excel-cod.xlsx
+++ b/01-carga-excel/sqlite/docs/excel-cod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E08DCAC3-7FD5-4D7E-9412-48724040E25B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="10" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="10" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -2994,64 +2994,64 @@
     <t>RDL</t>
   </si>
   <si>
+    <t>Residente en los tres años inmediatamente anteriores a la solicitud , nacido en España =18 años  (art. 183.3.c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residente en los tres años inmediatamente anteriores a la solicitud, &gt;18 años y nacido en España </t>
+  </si>
+  <si>
+    <t>H2E003</t>
+  </si>
+  <si>
+    <t>RDM</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
-    <t>Residente en los tres años inmediatamente anteriores a la solicitud , nacido en España =18 años  (art. 183.3.c)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residente en los tres años inmediatamente anteriores a la solicitud, &gt;18 años y nacido en España </t>
-  </si>
-  <si>
-    <t>H2E003</t>
-  </si>
-  <si>
-    <t>RDM</t>
+    <t>(5) Extranjeros que hayan contribuido de forma notoria al progreso de España o a su proyección en el exterior  (art. 183.3.g)</t>
+  </si>
+  <si>
+    <t>Contribución notoria.OFICIO</t>
+  </si>
+  <si>
+    <t>N-CADUCIDAD</t>
+  </si>
+  <si>
+    <t>H2E008</t>
+  </si>
+  <si>
+    <t>RDN</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>(5) Extranjeros que hayan contribuido de forma notoria al progreso de España o a su proyección en el exterior  (art. 183.3.g)</t>
-  </si>
-  <si>
-    <t>Contribución notoria.OFICIO</t>
-  </si>
-  <si>
-    <t>N-CADUCIDAD</t>
-  </si>
-  <si>
-    <t>H2E008</t>
-  </si>
-  <si>
-    <t>RDN</t>
+    <t>Supuesto general 5 años de residencia legal continuada en España (art. 183.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supuesto general 5 años de residencia continuada en España </t>
+  </si>
+  <si>
+    <t>H2E000</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>Supuesto general 5 años de residencia legal continuada en España (art. 183.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supuesto general 5 años de residencia continuada en España </t>
-  </si>
-  <si>
-    <t>H2E000</t>
+    <t>Residente beneficiario de pensión contributiva de jubilación o  beneficiario de incapacidad permanente absoluta o gran invalidez  (art. 183.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residente beneficiario de pensión contributiva de jubilación o beneficiario de incapacidad permanente absoluta o gran invalidez </t>
+  </si>
+  <si>
+    <t>H2E002</t>
+  </si>
+  <si>
+    <t>RDP</t>
   </si>
   <si>
     <t>G</t>
-  </si>
-  <si>
-    <t>Residente beneficiario de pensión contributiva de jubilación o  beneficiario de incapacidad permanente absoluta o gran invalidez  (art. 183.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residente beneficiario de pensión contributiva de jubilación o beneficiario de incapacidad permanente absoluta o gran invalidez </t>
-  </si>
-  <si>
-    <t>H2E002</t>
-  </si>
-  <si>
-    <t>RDP</t>
   </si>
   <si>
     <t>IAEAAAAAKA</t>
@@ -3125,19 +3125,19 @@
     <t>2.7</t>
   </si>
   <si>
+    <t>Residente durante 5 años consecutivos inmediatamente anteriores  &gt;18 años bajo tutela de entidad (art. 183.3.e)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residente tutelado por entidad pública 5 años consecutivos inmediatamente anteriores a la mayoría de edad </t>
+  </si>
+  <si>
+    <t>H2E004</t>
+  </si>
+  <si>
+    <t>RDT</t>
+  </si>
+  <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>Residente durante 5 años consecutivos inmediatamente anteriores  &gt;18 años bajo tutela de entidad (art. 183.3.e)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residente tutelado por entidad pública 5 años consecutivos inmediatamente anteriores a la mayoría de edad </t>
-  </si>
-  <si>
-    <t>H2E004</t>
-  </si>
-  <si>
-    <t>RDT</t>
   </si>
   <si>
     <t xml:space="preserve">TITULAR de residencia de larga duración-UE en otro Estado miembro (art.179 ) </t>
@@ -4274,7 +4274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6432,19 +6432,19 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="4" max="4" width="57.5546875" customWidth="1"/>
-    <col min="5" max="5" width="47.88671875" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" customWidth="1"/>
     <col min="6" max="6" width="37" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="110.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="165.6">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="165.6">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="165.6">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="138" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="138">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="138" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="138">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="151.9">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="151.9">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="41.45">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -7029,7 +7029,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="41.45">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="124.15">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="124.15">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="82.9">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="82.9">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="55.15">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="55.15">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="55.15">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="55.15">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="82.9">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="82.9">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="41.45">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="151.9">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="41.45">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="82.9">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="41.45">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -8043,7 +8043,7 @@
       </c>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="55.15">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="41.45">
       <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="41.45">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="124.15">
       <c r="A29" s="4" t="s">
         <v>23</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="82.9">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="55.15">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="55.15">
       <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
@@ -8513,16 +8513,16 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.109375" customWidth="1"/>
-    <col min="5" max="5" width="45.5546875" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
-    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="110.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" ht="41.45">
       <c r="A2" s="161" t="s">
         <v>855</v>
       </c>
@@ -8766,7 +8766,7 @@
       <c r="AR2" s="147"/>
       <c r="AS2" s="147"/>
     </row>
-    <row r="3" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" ht="27.6">
       <c r="A3" s="161" t="s">
         <v>855</v>
       </c>
@@ -8873,7 +8873,7 @@
       <c r="AR3" s="147"/>
       <c r="AS3" s="147"/>
     </row>
-    <row r="4" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" ht="27.6">
       <c r="A4" s="161" t="s">
         <v>855</v>
       </c>
@@ -8980,7 +8980,7 @@
       <c r="AR4" s="147"/>
       <c r="AS4" s="147"/>
     </row>
-    <row r="5" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" ht="27.6">
       <c r="A5" s="161" t="s">
         <v>855</v>
       </c>
@@ -8992,10 +8992,10 @@
         <v>857</v>
       </c>
       <c r="E5" s="141" t="s">
+        <v>875</v>
+      </c>
+      <c r="F5" s="141" t="s">
         <v>876</v>
-      </c>
-      <c r="F5" s="141" t="s">
-        <v>877</v>
       </c>
       <c r="G5" s="162" t="s">
         <v>298</v>
@@ -9007,13 +9007,13 @@
         <v>131</v>
       </c>
       <c r="J5" s="163" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K5" s="147" t="s">
         <v>861</v>
       </c>
       <c r="L5" s="147" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="M5" s="162" t="s">
         <v>201</v>
@@ -9065,7 +9065,7 @@
         <v>856</v>
       </c>
       <c r="AF5" s="139" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="AG5" s="147" t="s">
         <v>209</v>
@@ -9089,7 +9089,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" ht="41.45">
       <c r="A6" s="161" t="s">
         <v>855</v>
       </c>
@@ -9101,10 +9101,10 @@
         <v>857</v>
       </c>
       <c r="E6" s="141" t="s">
+        <v>880</v>
+      </c>
+      <c r="F6" s="141" t="s">
         <v>881</v>
-      </c>
-      <c r="F6" s="141" t="s">
-        <v>882</v>
       </c>
       <c r="G6" s="162" t="s">
         <v>298</v>
@@ -9113,16 +9113,16 @@
         <v>215</v>
       </c>
       <c r="I6" s="147" t="s">
+        <v>882</v>
+      </c>
+      <c r="J6" s="163" t="s">
         <v>883</v>
-      </c>
-      <c r="J6" s="163" t="s">
-        <v>884</v>
       </c>
       <c r="K6" s="147" t="s">
         <v>861</v>
       </c>
       <c r="L6" s="147" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="M6" s="162" t="s">
         <v>201</v>
@@ -9174,7 +9174,7 @@
         <v>856</v>
       </c>
       <c r="AF6" s="139" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="AG6" s="147" t="s">
         <v>209</v>
@@ -9196,7 +9196,7 @@
       <c r="AR6" s="147"/>
       <c r="AS6" s="147"/>
     </row>
-    <row r="7" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" ht="27.6">
       <c r="A7" s="161" t="s">
         <v>855</v>
       </c>
@@ -9208,10 +9208,10 @@
         <v>857</v>
       </c>
       <c r="E7" s="141" t="s">
+        <v>886</v>
+      </c>
+      <c r="F7" s="141" t="s">
         <v>887</v>
-      </c>
-      <c r="F7" s="141" t="s">
-        <v>888</v>
       </c>
       <c r="G7" s="162" t="s">
         <v>298</v>
@@ -9223,7 +9223,7 @@
         <v>131</v>
       </c>
       <c r="J7" s="163" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="K7" s="147" t="s">
         <v>861</v>
@@ -9281,7 +9281,7 @@
         <v>856</v>
       </c>
       <c r="AF7" s="139" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="AG7" s="147" t="s">
         <v>209</v>
@@ -9303,7 +9303,7 @@
       <c r="AR7" s="147"/>
       <c r="AS7" s="147"/>
     </row>
-    <row r="8" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" ht="41.45">
       <c r="A8" s="161" t="s">
         <v>855</v>
       </c>
@@ -9315,10 +9315,10 @@
         <v>857</v>
       </c>
       <c r="E8" s="167" t="s">
+        <v>890</v>
+      </c>
+      <c r="F8" s="141" t="s">
         <v>891</v>
-      </c>
-      <c r="F8" s="141" t="s">
-        <v>892</v>
       </c>
       <c r="G8" s="162" t="s">
         <v>298</v>
@@ -9330,13 +9330,13 @@
         <v>131</v>
       </c>
       <c r="J8" s="163" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K8" s="147" t="s">
         <v>861</v>
       </c>
       <c r="L8" s="147" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="M8" s="162" t="s">
         <v>201</v>
@@ -9388,7 +9388,7 @@
         <v>856</v>
       </c>
       <c r="AF8" s="139" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="AG8" s="147" t="s">
         <v>209</v>
@@ -9410,7 +9410,7 @@
       <c r="AR8" s="147"/>
       <c r="AS8" s="147"/>
     </row>
-    <row r="9" spans="1:45" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" ht="55.15">
       <c r="A9" s="161" t="s">
         <v>855</v>
       </c>
@@ -9517,7 +9517,7 @@
       <c r="AR9" s="147"/>
       <c r="AS9" s="147"/>
     </row>
-    <row r="10" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" ht="41.45">
       <c r="A10" s="161" t="s">
         <v>855</v>
       </c>
@@ -9624,7 +9624,7 @@
       <c r="AR10" s="147"/>
       <c r="AS10" s="147"/>
     </row>
-    <row r="11" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" ht="41.45">
       <c r="A11" s="161" t="s">
         <v>855</v>
       </c>
@@ -9636,10 +9636,10 @@
         <v>857</v>
       </c>
       <c r="E11" s="141" t="s">
+        <v>907</v>
+      </c>
+      <c r="F11" s="141" t="s">
         <v>908</v>
-      </c>
-      <c r="F11" s="141" t="s">
-        <v>909</v>
       </c>
       <c r="G11" s="162" t="s">
         <v>298</v>
@@ -9651,13 +9651,13 @@
         <v>131</v>
       </c>
       <c r="J11" s="163" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="K11" s="147" t="s">
         <v>861</v>
       </c>
       <c r="L11" s="147" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="M11" s="162" t="s">
         <v>201</v>
@@ -9709,7 +9709,7 @@
         <v>856</v>
       </c>
       <c r="AF11" s="139" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="AG11" s="147" t="s">
         <v>209</v>
@@ -9731,7 +9731,7 @@
       <c r="AR11" s="147"/>
       <c r="AS11" s="147"/>
     </row>
-    <row r="12" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" ht="27.6">
       <c r="A12" s="161" t="s">
         <v>855</v>
       </c>
@@ -9838,7 +9838,7 @@
       <c r="AR12" s="147"/>
       <c r="AS12" s="147"/>
     </row>
-    <row r="13" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" ht="41.45">
       <c r="A13" s="161" t="s">
         <v>855</v>
       </c>
@@ -9945,7 +9945,7 @@
       <c r="AR13" s="147"/>
       <c r="AS13" s="147"/>
     </row>
-    <row r="14" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" ht="41.45">
       <c r="A14" s="161" t="s">
         <v>855</v>
       </c>
@@ -10030,7 +10030,7 @@
         <v>895</v>
       </c>
       <c r="AF14" s="139" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="AG14" s="147" t="s">
         <v>209</v>
@@ -10052,7 +10052,7 @@
       <c r="AR14" s="147"/>
       <c r="AS14" s="147"/>
     </row>
-    <row r="15" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" ht="41.45">
       <c r="A15" s="161" t="s">
         <v>855</v>
       </c>
@@ -10159,7 +10159,7 @@
       <c r="AR15" s="147"/>
       <c r="AS15" s="147"/>
     </row>
-    <row r="16" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" ht="41.45">
       <c r="A16" s="161" t="s">
         <v>855</v>
       </c>
@@ -10266,7 +10266,7 @@
       <c r="AR16" s="147"/>
       <c r="AS16" s="147"/>
     </row>
-    <row r="17" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" ht="41.45">
       <c r="A17" s="161" t="s">
         <v>855</v>
       </c>
@@ -10373,7 +10373,7 @@
       <c r="AR17" s="147"/>
       <c r="AS17" s="147"/>
     </row>
-    <row r="18" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" ht="41.45">
       <c r="A18" s="161" t="s">
         <v>855</v>
       </c>
@@ -10480,7 +10480,7 @@
       <c r="AR18" s="147"/>
       <c r="AS18" s="147"/>
     </row>
-    <row r="19" spans="1:45" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:45" ht="55.15">
       <c r="A19" s="161" t="s">
         <v>855</v>
       </c>
@@ -10587,7 +10587,7 @@
       <c r="AR19" s="147"/>
       <c r="AS19" s="147"/>
     </row>
-    <row r="20" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:45" ht="41.45">
       <c r="A20" s="161" t="s">
         <v>855</v>
       </c>
@@ -10672,7 +10672,7 @@
         <v>927</v>
       </c>
       <c r="AF20" s="139" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="AG20" s="147" t="s">
         <v>209</v>
@@ -10714,24 +10714,24 @@
   </sheetPr>
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="48.6640625" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="13" max="13" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
     <col min="31" max="31" width="13" customWidth="1"/>
-    <col min="34" max="34" width="39.44140625" customWidth="1"/>
-    <col min="35" max="35" width="14.5546875" customWidth="1"/>
+    <col min="34" max="34" width="39.42578125" customWidth="1"/>
+    <col min="35" max="35" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="41.45">
       <c r="A1" s="275" t="s">
         <v>953</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36">
       <c r="A2" s="280" t="s">
         <v>976</v>
       </c>
@@ -10913,7 +10913,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36">
       <c r="A3" s="280" t="s">
         <v>976</v>
       </c>
@@ -10982,7 +10982,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36">
       <c r="A4" s="280" t="s">
         <v>976</v>
       </c>
@@ -11053,7 +11053,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36">
       <c r="A5" s="280" t="s">
         <v>976</v>
       </c>
@@ -11141,17 +11141,17 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.45"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="182" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="182" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="172" customFormat="1" ht="110.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" s="172" customFormat="1" ht="110.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11332,7 +11332,7 @@
       <c r="CJ1" s="178"/>
       <c r="CK1" s="178"/>
     </row>
-    <row r="2" spans="1:89" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:89" ht="41.45">
       <c r="A2" s="1" t="s">
         <v>1004</v>
       </c>
@@ -11428,7 +11428,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="3" spans="1:89" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:89" ht="41.45">
       <c r="A3" s="1" t="s">
         <v>1004</v>
       </c>
@@ -11524,7 +11524,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:89" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:89" ht="41.45">
       <c r="A4" s="1" t="s">
         <v>1004</v>
       </c>
@@ -11618,7 +11618,7 @@
       </c>
       <c r="AH4" s="31"/>
     </row>
-    <row r="5" spans="1:89" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:89" ht="41.45">
       <c r="A5" s="1" t="s">
         <v>1004</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>1005</v>
       </c>
       <c r="C5" s="179" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>1006</v>
@@ -11705,14 +11705,14 @@
         <v>1005</v>
       </c>
       <c r="AF5" s="181" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="AG5" s="34" t="s">
         <v>209</v>
       </c>
       <c r="AH5" s="31"/>
     </row>
-    <row r="6" spans="1:89" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:89" ht="41.45">
       <c r="A6" s="1" t="s">
         <v>1004</v>
       </c>
@@ -11808,7 +11808,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:89" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:89" ht="41.45">
       <c r="A7" s="1" t="s">
         <v>1004</v>
       </c>
@@ -11925,13 +11925,13 @@
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="50.88671875" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="110.45">
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
@@ -12068,7 +12068,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" ht="41.45">
       <c r="A2" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12173,7 +12173,7 @@
       <c r="AR2" s="180"/>
       <c r="AS2" s="180"/>
     </row>
-    <row r="3" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" ht="41.45">
       <c r="A3" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12278,7 +12278,7 @@
       <c r="AR3" s="180"/>
       <c r="AS3" s="180"/>
     </row>
-    <row r="4" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" ht="39.6">
       <c r="A4" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12383,7 +12383,7 @@
       <c r="AR4" s="180"/>
       <c r="AS4" s="180"/>
     </row>
-    <row r="5" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" ht="39.6">
       <c r="A5" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12488,7 +12488,7 @@
       <c r="AR5" s="180"/>
       <c r="AS5" s="180"/>
     </row>
-    <row r="6" spans="1:45" ht="66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" ht="66">
       <c r="A6" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12593,7 +12593,7 @@
       <c r="AR6" s="180"/>
       <c r="AS6" s="180"/>
     </row>
-    <row r="7" spans="1:45" ht="66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" ht="66">
       <c r="A7" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12698,7 +12698,7 @@
       <c r="AR7" s="180"/>
       <c r="AS7" s="180"/>
     </row>
-    <row r="8" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" ht="41.45">
       <c r="A8" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12803,7 +12803,7 @@
       <c r="AR8" s="180"/>
       <c r="AS8" s="180"/>
     </row>
-    <row r="9" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" ht="41.45">
       <c r="A9" s="184" t="s">
         <v>1034</v>
       </c>
@@ -12908,7 +12908,7 @@
       <c r="AR9" s="180"/>
       <c r="AS9" s="180"/>
     </row>
-    <row r="10" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" ht="39.6">
       <c r="A10" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13013,7 +13013,7 @@
       <c r="AR10" s="180"/>
       <c r="AS10" s="180"/>
     </row>
-    <row r="11" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" ht="41.45">
       <c r="A11" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13118,7 +13118,7 @@
       <c r="AR11" s="180"/>
       <c r="AS11" s="180"/>
     </row>
-    <row r="12" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" ht="39.6">
       <c r="A12" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13223,7 +13223,7 @@
       <c r="AR12" s="180"/>
       <c r="AS12" s="180"/>
     </row>
-    <row r="13" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" ht="39.6">
       <c r="A13" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13324,7 +13324,7 @@
       <c r="AR13" s="91"/>
       <c r="AS13" s="91"/>
     </row>
-    <row r="14" spans="1:45" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" ht="79.150000000000006">
       <c r="A14" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13431,7 +13431,7 @@
       <c r="AR14" s="180"/>
       <c r="AS14" s="180"/>
     </row>
-    <row r="15" spans="1:45" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" ht="57.6">
       <c r="A15" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13538,7 +13538,7 @@
       <c r="AR15" s="180"/>
       <c r="AS15" s="180"/>
     </row>
-    <row r="16" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" ht="39.6">
       <c r="A16" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13643,7 +13643,7 @@
       <c r="AR16" s="180"/>
       <c r="AS16" s="180"/>
     </row>
-    <row r="17" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" ht="39.6">
       <c r="A17" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13748,7 +13748,7 @@
       <c r="AR17" s="180"/>
       <c r="AS17" s="180"/>
     </row>
-    <row r="18" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" ht="39.6">
       <c r="A18" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13853,7 +13853,7 @@
       <c r="AR18" s="180"/>
       <c r="AS18" s="180"/>
     </row>
-    <row r="19" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:45" ht="39.6">
       <c r="A19" s="184" t="s">
         <v>1034</v>
       </c>
@@ -13958,7 +13958,7 @@
       <c r="AR19" s="180"/>
       <c r="AS19" s="180"/>
     </row>
-    <row r="20" spans="1:45" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:45" ht="39.6">
       <c r="A20" s="184" t="s">
         <v>1034</v>
       </c>
@@ -14063,7 +14063,7 @@
       <c r="AR20" s="180"/>
       <c r="AS20" s="180"/>
     </row>
-    <row r="21" spans="1:45" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:45" ht="55.15">
       <c r="A21" s="184" t="s">
         <v>1034</v>
       </c>
@@ -14146,7 +14146,7 @@
         <v>1134</v>
       </c>
       <c r="AF21" s="34" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="AG21" s="34" t="s">
         <v>1135</v>
@@ -14168,7 +14168,7 @@
       <c r="AR21" s="34"/>
       <c r="AS21" s="34"/>
     </row>
-    <row r="22" spans="1:45" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:45" ht="55.15">
       <c r="A22" s="184" t="s">
         <v>1034</v>
       </c>
@@ -14251,7 +14251,7 @@
         <v>1134</v>
       </c>
       <c r="AF22" s="34" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="AG22" s="34" t="s">
         <v>1135</v>
@@ -14273,7 +14273,7 @@
       <c r="AR22" s="34"/>
       <c r="AS22" s="34"/>
     </row>
-    <row r="23" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:45" ht="27.6">
       <c r="A23" s="203" t="s">
         <v>1143</v>
       </c>
@@ -14334,7 +14334,7 @@
       <c r="AR23" s="34"/>
       <c r="AS23" s="34"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:45">
       <c r="A24" s="203" t="s">
         <v>1143</v>
       </c>
@@ -14395,7 +14395,7 @@
       <c r="AR24" s="34"/>
       <c r="AS24" s="34"/>
     </row>
-    <row r="25" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:45" ht="27.6">
       <c r="A25" s="203" t="s">
         <v>1143</v>
       </c>
@@ -14456,7 +14456,7 @@
       <c r="AR25" s="34"/>
       <c r="AS25" s="34"/>
     </row>
-    <row r="26" spans="1:45" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:45" ht="55.15">
       <c r="A26" s="203" t="s">
         <v>1143</v>
       </c>
@@ -14578,18 +14578,18 @@
       <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="3" width="10.88671875" style="182"/>
-    <col min="4" max="4" width="46.88671875" style="182" customWidth="1"/>
-    <col min="5" max="5" width="51.109375" style="272" customWidth="1"/>
-    <col min="6" max="6" width="44.44140625" style="182" customWidth="1"/>
-    <col min="7" max="13" width="10.88671875" style="182"/>
-    <col min="14" max="15" width="10.88671875" style="273"/>
-    <col min="16" max="16384" width="10.88671875" style="182"/>
+    <col min="1" max="3" width="10.85546875" style="182"/>
+    <col min="4" max="4" width="46.85546875" style="182" customWidth="1"/>
+    <col min="5" max="5" width="51.140625" style="272" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" style="182" customWidth="1"/>
+    <col min="7" max="13" width="10.85546875" style="182"/>
+    <col min="14" max="15" width="10.85546875" style="273"/>
+    <col min="16" max="16384" width="10.85546875" style="182"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" customFormat="1" ht="110.45">
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
@@ -14726,7 +14726,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A2" s="305" t="s">
         <v>1160</v>
       </c>
@@ -14837,7 +14837,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A3" s="305" t="s">
         <v>1160</v>
       </c>
@@ -14948,7 +14948,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A4" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15059,7 +15059,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A5" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15170,7 +15170,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A6" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15281,7 +15281,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A7" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15392,7 +15392,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:45" s="324" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" s="324" customFormat="1" ht="41.45">
       <c r="A8" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15503,7 +15503,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A9" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15614,7 +15614,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="10" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A10" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15725,7 +15725,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="11" spans="1:45" s="327" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" s="327" customFormat="1" ht="41.45">
       <c r="A11" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15820,7 +15820,7 @@
       <c r="AR11" s="306"/>
       <c r="AS11" s="306"/>
     </row>
-    <row r="12" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A12" s="305" t="s">
         <v>1160</v>
       </c>
@@ -15917,7 +15917,7 @@
       <c r="AR12" s="306"/>
       <c r="AS12" s="306"/>
     </row>
-    <row r="13" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A13" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16012,7 +16012,7 @@
       <c r="AR13" s="306"/>
       <c r="AS13" s="306"/>
     </row>
-    <row r="14" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A14" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16109,7 +16109,7 @@
       <c r="AR14" s="306"/>
       <c r="AS14" s="306"/>
     </row>
-    <row r="15" spans="1:45" s="285" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" s="285" customFormat="1" ht="27.6">
       <c r="A15" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16202,7 +16202,7 @@
       <c r="AR15" s="306"/>
       <c r="AS15" s="306"/>
     </row>
-    <row r="16" spans="1:45" s="285" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" s="285" customFormat="1" ht="41.45">
       <c r="A16" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16313,7 +16313,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="17" spans="1:45" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" customFormat="1" ht="41.45">
       <c r="A17" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16410,7 +16410,7 @@
       <c r="AR17" s="306"/>
       <c r="AS17" s="306"/>
     </row>
-    <row r="18" spans="1:45" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" customFormat="1" ht="27.6">
       <c r="A18" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16503,7 +16503,7 @@
       <c r="AR18" s="306"/>
       <c r="AS18" s="306"/>
     </row>
-    <row r="19" spans="1:45" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:45" customFormat="1" ht="41.45">
       <c r="A19" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16598,7 +16598,7 @@
       <c r="AR19" s="306"/>
       <c r="AS19" s="306"/>
     </row>
-    <row r="20" spans="1:45" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:45" customFormat="1" ht="41.45">
       <c r="A20" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16691,7 +16691,7 @@
       <c r="AR20" s="306"/>
       <c r="AS20" s="306"/>
     </row>
-    <row r="21" spans="1:45" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:45" customFormat="1" ht="41.45">
       <c r="A21" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16802,7 +16802,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="22" spans="1:45" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:45" customFormat="1" ht="41.45">
       <c r="A22" s="305" t="s">
         <v>1160</v>
       </c>
@@ -16913,7 +16913,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="23" spans="1:45" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:45" customFormat="1" ht="41.45">
       <c r="A23" s="305" t="s">
         <v>1160</v>
       </c>
@@ -17022,7 +17022,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="24" spans="1:45" s="316" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:45" s="316" customFormat="1" ht="41.45">
       <c r="A24" s="305" t="s">
         <v>1160</v>
       </c>
@@ -17135,7 +17135,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="25" spans="1:45" s="316" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:45" s="316" customFormat="1" ht="27.6">
       <c r="A25" s="305" t="s">
         <v>1160</v>
       </c>
@@ -17291,9 +17291,9 @@
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:89" s="172" customFormat="1" ht="55.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" s="172" customFormat="1" ht="55.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17474,7 +17474,7 @@
       <c r="CJ1" s="178"/>
       <c r="CK1" s="178"/>
     </row>
-    <row r="2" spans="1:89" s="33" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A2" s="1" t="s">
         <v>1258</v>
       </c>
@@ -17565,7 +17565,7 @@
       <c r="BL2" s="76"/>
       <c r="BM2" s="174"/>
     </row>
-    <row r="3" spans="1:89" s="33" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A3" s="1" t="s">
         <v>1258</v>
       </c>
@@ -17656,7 +17656,7 @@
       <c r="BL3" s="76"/>
       <c r="BM3" s="174"/>
     </row>
-    <row r="4" spans="1:89" s="33" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A4" s="1" t="s">
         <v>1258</v>
       </c>
@@ -17747,7 +17747,7 @@
       <c r="BL4" s="76"/>
       <c r="BM4" s="174"/>
     </row>
-    <row r="5" spans="1:89" s="33" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A5" s="1" t="s">
         <v>1258</v>
       </c>
@@ -17855,18 +17855,18 @@
   </sheetPr>
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
     <col min="4" max="4" width="58" customWidth="1"/>
-    <col min="6" max="6" width="53.44140625" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="110.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18003,7 +18003,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" ht="41.45">
       <c r="A2" s="1" t="s">
         <v>194</v>
       </c>
@@ -18089,7 +18089,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" ht="41.45">
       <c r="A3" s="1" t="s">
         <v>194</v>
       </c>
@@ -18175,7 +18175,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" ht="27.6">
       <c r="A4" s="1" t="s">
         <v>194</v>
       </c>
@@ -18261,7 +18261,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" ht="27.6">
       <c r="A5" s="1" t="s">
         <v>194</v>
       </c>
@@ -18364,35 +18364,35 @@
   </sheetPr>
   <dimension ref="A1:CK15"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="4" max="4" width="55.109375" customWidth="1"/>
+    <col min="4" max="4" width="55.140625" customWidth="1"/>
     <col min="5" max="5" width="66" customWidth="1"/>
-    <col min="6" max="6" width="63.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" customWidth="1"/>
-    <col min="19" max="19" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="63.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" customWidth="1"/>
     <col min="20" max="20" width="13" customWidth="1"/>
-    <col min="21" max="21" width="15.33203125" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
-    <col min="23" max="23" width="15.88671875" customWidth="1"/>
-    <col min="24" max="24" width="14.109375" customWidth="1"/>
-    <col min="26" max="26" width="19.109375" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" customWidth="1"/>
     <col min="27" max="27" width="17" customWidth="1"/>
-    <col min="28" max="28" width="13.6640625" customWidth="1"/>
-    <col min="30" max="30" width="16.44140625" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="172" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" s="172" customFormat="1" ht="25.5" customHeight="1">
       <c r="A1" s="255" t="s">
         <v>0</v>
       </c>
@@ -18573,7 +18573,7 @@
       <c r="CJ1" s="178"/>
       <c r="CK1" s="178"/>
     </row>
-    <row r="2" spans="1:89" s="172" customFormat="1" ht="207" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:89" s="172" customFormat="1" ht="207">
       <c r="A2" s="1" t="s">
         <v>225</v>
       </c>
@@ -18718,7 +18718,7 @@
       <c r="CJ2" s="178"/>
       <c r="CK2" s="178"/>
     </row>
-    <row r="3" spans="1:89" s="172" customFormat="1" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:89" s="172" customFormat="1" ht="27.6">
       <c r="A3" s="1" t="s">
         <v>225</v>
       </c>
@@ -18861,7 +18861,7 @@
       <c r="CJ3" s="178"/>
       <c r="CK3" s="178"/>
     </row>
-    <row r="4" spans="1:89" s="172" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:89" s="172" customFormat="1" ht="56.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>225</v>
       </c>
@@ -19002,7 +19002,7 @@
       <c r="CJ4" s="178"/>
       <c r="CK4" s="178"/>
     </row>
-    <row r="5" spans="1:89" s="172" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:89" s="172" customFormat="1" ht="71.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>225</v>
       </c>
@@ -19143,7 +19143,7 @@
       <c r="CJ5" s="178"/>
       <c r="CK5" s="178"/>
     </row>
-    <row r="6" spans="1:89" s="172" customFormat="1" ht="124.2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:89" s="172" customFormat="1" ht="124.15">
       <c r="A6" s="1" t="s">
         <v>225</v>
       </c>
@@ -19288,7 +19288,7 @@
       <c r="CJ6" s="178"/>
       <c r="CK6" s="178"/>
     </row>
-    <row r="7" spans="1:89" s="172" customFormat="1" ht="55.2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:89" s="172" customFormat="1" ht="55.15">
       <c r="A7" s="1" t="s">
         <v>225</v>
       </c>
@@ -19433,7 +19433,7 @@
       <c r="CJ7" s="178"/>
       <c r="CK7" s="178"/>
     </row>
-    <row r="8" spans="1:89" s="172" customFormat="1" ht="82.8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:89" s="172" customFormat="1" ht="82.9">
       <c r="A8" s="1" t="s">
         <v>225</v>
       </c>
@@ -19578,7 +19578,7 @@
       <c r="CJ8" s="178"/>
       <c r="CK8" s="178"/>
     </row>
-    <row r="9" spans="1:89" s="172" customFormat="1" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:89" s="172" customFormat="1" ht="27.6">
       <c r="A9" s="1" t="s">
         <v>225</v>
       </c>
@@ -19721,7 +19721,7 @@
       <c r="CJ9" s="178"/>
       <c r="CK9" s="178"/>
     </row>
-    <row r="10" spans="1:89" s="172" customFormat="1" ht="69" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:89" s="172" customFormat="1" ht="69">
       <c r="A10" s="1" t="s">
         <v>225</v>
       </c>
@@ -19866,7 +19866,7 @@
       <c r="CJ10" s="178"/>
       <c r="CK10" s="178"/>
     </row>
-    <row r="11" spans="1:89" s="172" customFormat="1" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:89" s="172" customFormat="1" ht="27.6">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -20001,7 +20001,7 @@
       <c r="CJ11" s="178"/>
       <c r="CK11" s="178"/>
     </row>
-    <row r="12" spans="1:89" s="172" customFormat="1" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:89" s="172" customFormat="1" ht="27.6">
       <c r="A12" s="1" t="s">
         <v>225</v>
       </c>
@@ -20138,7 +20138,7 @@
       <c r="CJ12" s="178"/>
       <c r="CK12" s="178"/>
     </row>
-    <row r="13" spans="1:89" s="172" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:89" s="172" customFormat="1" ht="147.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>225</v>
       </c>
@@ -20283,7 +20283,7 @@
       <c r="CJ13" s="178"/>
       <c r="CK13" s="178"/>
     </row>
-    <row r="14" spans="1:89" s="172" customFormat="1" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:89" s="172" customFormat="1" ht="27.6">
       <c r="A14" s="1" t="s">
         <v>225</v>
       </c>
@@ -20426,7 +20426,7 @@
       <c r="CJ14" s="178"/>
       <c r="CK14" s="178"/>
     </row>
-    <row r="15" spans="1:89" s="172" customFormat="1" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:89" s="172" customFormat="1" ht="27.6">
       <c r="A15" s="1" t="s">
         <v>225</v>
       </c>
@@ -20606,27 +20606,27 @@
       <selection activeCell="L23" sqref="K23:L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="252"/>
-    <col min="2" max="2" width="16.33203125" style="252" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="252" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" style="252" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="252" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" style="252" customWidth="1"/>
-    <col min="7" max="16" width="11.44140625" style="252"/>
-    <col min="17" max="17" width="11.44140625" style="254"/>
-    <col min="18" max="18" width="11.44140625" style="252"/>
+    <col min="1" max="1" width="11.42578125" style="252"/>
+    <col min="2" max="2" width="16.28515625" style="252" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="252" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="252" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="252" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" style="252" customWidth="1"/>
+    <col min="7" max="16" width="11.42578125" style="252"/>
+    <col min="17" max="17" width="11.42578125" style="254"/>
+    <col min="18" max="18" width="11.42578125" style="252"/>
     <col min="19" max="19" width="14" style="254" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="254"/>
-    <col min="21" max="21" width="12.5546875" style="254" customWidth="1"/>
-    <col min="22" max="22" width="11.44140625" style="254"/>
-    <col min="23" max="30" width="11.44140625" style="252"/>
-    <col min="31" max="31" width="16.5546875" style="252" customWidth="1"/>
-    <col min="32" max="16384" width="11.44140625" style="252"/>
+    <col min="20" max="20" width="11.42578125" style="254"/>
+    <col min="21" max="21" width="12.5703125" style="254" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="254"/>
+    <col min="23" max="30" width="11.42578125" style="252"/>
+    <col min="31" max="31" width="16.5703125" style="252" customWidth="1"/>
+    <col min="32" max="16384" width="11.42578125" style="252"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="218" customFormat="1" ht="110.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" s="218" customFormat="1" ht="110.45">
       <c r="A1" s="206" t="s">
         <v>0</v>
       </c>
@@ -20807,7 +20807,7 @@
       <c r="CJ1" s="217"/>
       <c r="CK1" s="217"/>
     </row>
-    <row r="2" spans="1:89" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:89" s="228" customFormat="1" ht="55.15">
       <c r="A2" s="224" t="s">
         <v>318</v>
       </c>
@@ -20940,7 +20940,7 @@
       <c r="BL2" s="226"/>
       <c r="BM2" s="227"/>
     </row>
-    <row r="3" spans="1:89" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:89" s="228" customFormat="1" ht="55.15">
       <c r="A3" s="224" t="s">
         <v>318</v>
       </c>
@@ -21073,7 +21073,7 @@
       <c r="BL3" s="226"/>
       <c r="BM3" s="227"/>
     </row>
-    <row r="4" spans="1:89" s="228" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:89" s="228" customFormat="1" ht="69">
       <c r="A4" s="224" t="s">
         <v>318</v>
       </c>
@@ -21206,7 +21206,7 @@
       <c r="BL4" s="226"/>
       <c r="BM4" s="227"/>
     </row>
-    <row r="5" spans="1:89" s="228" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:89" s="228" customFormat="1" ht="69">
       <c r="A5" s="224" t="s">
         <v>318</v>
       </c>
@@ -21339,7 +21339,7 @@
       <c r="BL5" s="226"/>
       <c r="BM5" s="227"/>
     </row>
-    <row r="6" spans="1:89" s="228" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:89" s="228" customFormat="1" ht="124.15">
       <c r="A6" s="224" t="s">
         <v>318</v>
       </c>
@@ -21474,7 +21474,7 @@
       <c r="BL6" s="226"/>
       <c r="BM6" s="227"/>
     </row>
-    <row r="7" spans="1:89" s="228" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:89" s="228" customFormat="1" ht="124.15">
       <c r="A7" s="224" t="s">
         <v>318</v>
       </c>
@@ -21609,7 +21609,7 @@
       <c r="BL7" s="226"/>
       <c r="BM7" s="227"/>
     </row>
-    <row r="8" spans="1:89" s="228" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:89" s="228" customFormat="1" ht="124.15">
       <c r="A8" s="224" t="s">
         <v>318</v>
       </c>
@@ -21744,7 +21744,7 @@
       <c r="BL8" s="226"/>
       <c r="BM8" s="227"/>
     </row>
-    <row r="9" spans="1:89" s="228" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:89" s="228" customFormat="1" ht="124.15">
       <c r="A9" s="224" t="s">
         <v>318</v>
       </c>
@@ -21879,7 +21879,7 @@
       <c r="BL9" s="226"/>
       <c r="BM9" s="227"/>
     </row>
-    <row r="10" spans="1:89" s="247" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:89" s="247" customFormat="1" ht="55.15">
       <c r="A10" s="224" t="s">
         <v>318</v>
       </c>
@@ -22031,7 +22031,7 @@
       <c r="CI10" s="238"/>
       <c r="CJ10" s="238"/>
     </row>
-    <row r="11" spans="1:89" s="247" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:89" s="247" customFormat="1" ht="55.15">
       <c r="A11" s="224" t="s">
         <v>318</v>
       </c>
@@ -22183,7 +22183,7 @@
       <c r="CI11" s="238"/>
       <c r="CJ11" s="238"/>
     </row>
-    <row r="12" spans="1:89" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:89" s="228" customFormat="1" ht="55.15">
       <c r="A12" s="224" t="s">
         <v>318</v>
       </c>
@@ -22316,7 +22316,7 @@
       <c r="BL12" s="226"/>
       <c r="BM12" s="227"/>
     </row>
-    <row r="13" spans="1:89" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:89" s="228" customFormat="1" ht="55.15">
       <c r="A13" s="224" t="s">
         <v>318</v>
       </c>
@@ -22449,7 +22449,7 @@
       <c r="BL13" s="226"/>
       <c r="BM13" s="227"/>
     </row>
-    <row r="14" spans="1:89" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:89" s="228" customFormat="1" ht="55.15">
       <c r="A14" s="224" t="s">
         <v>318</v>
       </c>
@@ -22578,7 +22578,7 @@
       <c r="BL14" s="226"/>
       <c r="BM14" s="227"/>
     </row>
-    <row r="15" spans="1:89" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:89" s="228" customFormat="1" ht="55.15">
       <c r="A15" s="224" t="s">
         <v>318</v>
       </c>
@@ -22707,7 +22707,7 @@
       <c r="BL15" s="226"/>
       <c r="BM15" s="227"/>
     </row>
-    <row r="16" spans="1:89" s="228" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:89" s="228" customFormat="1" ht="110.45">
       <c r="A16" s="224" t="s">
         <v>318</v>
       </c>
@@ -22832,7 +22832,7 @@
       <c r="BL16" s="226"/>
       <c r="BM16" s="227"/>
     </row>
-    <row r="17" spans="1:88" s="228" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:88" s="228" customFormat="1" ht="96.6">
       <c r="A17" s="224" t="s">
         <v>318</v>
       </c>
@@ -22961,7 +22961,7 @@
       <c r="BL17" s="226"/>
       <c r="BM17" s="227"/>
     </row>
-    <row r="18" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A18" s="224" t="s">
         <v>407</v>
       </c>
@@ -23088,7 +23088,7 @@
       <c r="BL18" s="226"/>
       <c r="BM18" s="227"/>
     </row>
-    <row r="19" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A19" s="224" t="s">
         <v>318</v>
       </c>
@@ -23213,7 +23213,7 @@
       <c r="BL19" s="226"/>
       <c r="BM19" s="227"/>
     </row>
-    <row r="20" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A20" s="224" t="s">
         <v>318</v>
       </c>
@@ -23338,7 +23338,7 @@
       <c r="BL20" s="226"/>
       <c r="BM20" s="227"/>
     </row>
-    <row r="21" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A21" s="224" t="s">
         <v>318</v>
       </c>
@@ -23463,7 +23463,7 @@
       <c r="BL21" s="226"/>
       <c r="BM21" s="227"/>
     </row>
-    <row r="22" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A22" s="224" t="s">
         <v>318</v>
       </c>
@@ -23588,7 +23588,7 @@
       <c r="BL22" s="226"/>
       <c r="BM22" s="227"/>
     </row>
-    <row r="23" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A23" s="224" t="s">
         <v>318</v>
       </c>
@@ -23719,7 +23719,7 @@
       <c r="BL23" s="226"/>
       <c r="BM23" s="227"/>
     </row>
-    <row r="24" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A24" s="224" t="s">
         <v>318</v>
       </c>
@@ -23850,7 +23850,7 @@
       <c r="BL24" s="226"/>
       <c r="BM24" s="227"/>
     </row>
-    <row r="25" spans="1:88" s="247" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:88" s="247" customFormat="1" ht="55.15">
       <c r="A25" s="224" t="s">
         <v>318</v>
       </c>
@@ -24004,7 +24004,7 @@
       <c r="CI25" s="238"/>
       <c r="CJ25" s="238"/>
     </row>
-    <row r="26" spans="1:88" s="247" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:88" s="247" customFormat="1" ht="55.15">
       <c r="A26" s="224" t="s">
         <v>318</v>
       </c>
@@ -24158,7 +24158,7 @@
       <c r="CI26" s="238"/>
       <c r="CJ26" s="238"/>
     </row>
-    <row r="27" spans="1:88" s="228" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:88" s="228" customFormat="1" ht="55.15">
       <c r="A27" s="224" t="s">
         <v>407</v>
       </c>
@@ -24283,7 +24283,7 @@
       <c r="BL27" s="226"/>
       <c r="BM27" s="227"/>
     </row>
-    <row r="28" spans="1:88" s="228" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:88" s="228" customFormat="1" ht="124.15">
       <c r="A28" s="224" t="s">
         <v>318</v>
       </c>
@@ -24410,7 +24410,7 @@
       <c r="BL28" s="226"/>
       <c r="BM28" s="227"/>
     </row>
-    <row r="29" spans="1:88" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:88" ht="55.15">
       <c r="A29" s="248" t="s">
         <v>318</v>
       </c>
@@ -24523,7 +24523,7 @@
       <c r="AR29" s="224"/>
       <c r="AS29" s="224"/>
     </row>
-    <row r="30" spans="1:88" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:88" ht="55.15">
       <c r="A30" s="248" t="s">
         <v>318</v>
       </c>
@@ -24655,15 +24655,15 @@
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="5" max="5" width="60.44140625" customWidth="1"/>
-    <col min="6" max="6" width="53.44140625" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="60.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:89" ht="82.9">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -24800,7 +24800,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:89" s="60" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:89" s="60" customFormat="1" ht="41.45">
       <c r="A2" s="40" t="s">
         <v>486</v>
       </c>
@@ -24931,7 +24931,7 @@
       <c r="CJ2" s="59"/>
       <c r="CK2" s="59"/>
     </row>
-    <row r="3" spans="1:89" s="60" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:89" s="60" customFormat="1" ht="41.45">
       <c r="A3" s="40" t="s">
         <v>486</v>
       </c>
@@ -25058,7 +25058,7 @@
       <c r="CJ3" s="59"/>
       <c r="CK3" s="59"/>
     </row>
-    <row r="4" spans="1:89" s="60" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:89" s="60" customFormat="1" ht="41.45">
       <c r="A4" s="40" t="s">
         <v>486</v>
       </c>
@@ -25189,7 +25189,7 @@
       <c r="CJ4" s="59"/>
       <c r="CK4" s="59"/>
     </row>
-    <row r="5" spans="1:89" s="60" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:89" s="60" customFormat="1" ht="41.45">
       <c r="A5" s="40" t="s">
         <v>486</v>
       </c>
@@ -25316,7 +25316,7 @@
       <c r="CJ5" s="59"/>
       <c r="CK5" s="59"/>
     </row>
-    <row r="6" spans="1:89" s="60" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:89" s="60" customFormat="1" ht="69">
       <c r="A6" s="40" t="s">
         <v>486</v>
       </c>
@@ -25447,7 +25447,7 @@
       <c r="CJ6" s="59"/>
       <c r="CK6" s="59"/>
     </row>
-    <row r="7" spans="1:89" s="60" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:89" s="60" customFormat="1" ht="27.6">
       <c r="A7" s="40" t="s">
         <v>486</v>
       </c>
@@ -25576,7 +25576,7 @@
       <c r="CJ7" s="59"/>
       <c r="CK7" s="59"/>
     </row>
-    <row r="8" spans="1:89" s="60" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:89" s="60" customFormat="1" ht="27.6">
       <c r="A8" s="40" t="s">
         <v>486</v>
       </c>
@@ -25703,7 +25703,7 @@
       <c r="CJ8" s="59"/>
       <c r="CK8" s="59"/>
     </row>
-    <row r="9" spans="1:89" s="60" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:89" s="60" customFormat="1" ht="69">
       <c r="A9" s="40" t="s">
         <v>486</v>
       </c>
@@ -25857,16 +25857,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33.44140625" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="77" customFormat="1" ht="55.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:87" s="77" customFormat="1" ht="55.15">
       <c r="A1" s="64" t="s">
         <v>529</v>
       </c>
@@ -26045,7 +26045,7 @@
       <c r="CH1" s="76"/>
       <c r="CI1" s="76"/>
     </row>
-    <row r="2" spans="1:87" s="86" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:87" s="86" customFormat="1" ht="27.6">
       <c r="A2" s="78" t="s">
         <v>547</v>
       </c>
@@ -26163,7 +26163,7 @@
       <c r="BQ2" s="85"/>
       <c r="BR2" s="85"/>
     </row>
-    <row r="3" spans="1:87" s="86" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:87" s="86" customFormat="1" ht="41.45">
       <c r="A3" s="87" t="s">
         <v>547</v>
       </c>
@@ -26256,7 +26256,7 @@
       <c r="AR3" s="89"/>
       <c r="AS3" s="89"/>
     </row>
-    <row r="4" spans="1:87" s="86" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:87" s="86" customFormat="1" ht="41.45">
       <c r="A4" s="92" t="s">
         <v>547</v>
       </c>
@@ -26347,7 +26347,7 @@
       <c r="AR4" s="89"/>
       <c r="AS4" s="89"/>
     </row>
-    <row r="5" spans="1:87" s="86" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:87" s="86" customFormat="1" ht="41.45">
       <c r="A5" s="92" t="s">
         <v>547</v>
       </c>
@@ -26434,7 +26434,7 @@
       <c r="AR5" s="89"/>
       <c r="AS5" s="89"/>
     </row>
-    <row r="6" spans="1:87" s="86" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:87" s="86" customFormat="1" ht="41.45">
       <c r="A6" s="92" t="s">
         <v>547</v>
       </c>
@@ -26527,7 +26527,7 @@
       <c r="AR6" s="89"/>
       <c r="AS6" s="89"/>
     </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:87">
       <c r="F7" s="103"/>
     </row>
   </sheetData>
@@ -26551,20 +26551,20 @@
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="3" width="11.44140625" style="127"/>
-    <col min="4" max="4" width="56.5546875" style="127" customWidth="1"/>
-    <col min="5" max="5" width="50.109375" style="127" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" style="127" customWidth="1"/>
-    <col min="7" max="8" width="11.44140625" style="127"/>
-    <col min="9" max="29" width="11.44140625" style="128"/>
-    <col min="30" max="30" width="13.6640625" style="129" customWidth="1"/>
-    <col min="31" max="45" width="11.44140625" style="128"/>
-    <col min="46" max="16384" width="11.44140625" style="111"/>
+    <col min="1" max="3" width="11.42578125" style="127"/>
+    <col min="4" max="4" width="56.5703125" style="127" customWidth="1"/>
+    <col min="5" max="5" width="50.140625" style="127" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="127" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" style="127"/>
+    <col min="9" max="29" width="11.42578125" style="128"/>
+    <col min="30" max="30" width="13.7109375" style="129" customWidth="1"/>
+    <col min="31" max="45" width="11.42578125" style="128"/>
+    <col min="46" max="16384" width="11.42578125" style="111"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="110.45">
       <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
@@ -26701,7 +26701,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="121" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" s="121" customFormat="1" ht="41.45">
       <c r="A2" s="104" t="s">
         <v>586</v>
       </c>
@@ -26794,7 +26794,7 @@
       <c r="AR2" s="118"/>
       <c r="AS2" s="118"/>
     </row>
-    <row r="3" spans="1:45" s="121" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" s="121" customFormat="1">
       <c r="A3" s="104" t="s">
         <v>586</v>
       </c>
@@ -26865,7 +26865,7 @@
       <c r="AR3" s="118"/>
       <c r="AS3" s="118"/>
     </row>
-    <row r="4" spans="1:45" s="121" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" s="121" customFormat="1" ht="55.15">
       <c r="A4" s="104" t="s">
         <v>586</v>
       </c>
@@ -26958,7 +26958,7 @@
       <c r="AR4" s="118"/>
       <c r="AS4" s="118"/>
     </row>
-    <row r="5" spans="1:45" s="121" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" s="121" customFormat="1" ht="55.15">
       <c r="A5" s="104" t="s">
         <v>586</v>
       </c>
@@ -27051,7 +27051,7 @@
       <c r="AR5" s="118"/>
       <c r="AS5" s="118"/>
     </row>
-    <row r="6" spans="1:45" s="121" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" s="121" customFormat="1" ht="41.45">
       <c r="A6" s="104" t="s">
         <v>586</v>
       </c>
@@ -27140,7 +27140,7 @@
       <c r="AR6" s="118"/>
       <c r="AS6" s="118"/>
     </row>
-    <row r="7" spans="1:45" s="121" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" s="121" customFormat="1" ht="41.45">
       <c r="A7" s="104" t="s">
         <v>586</v>
       </c>
@@ -27231,7 +27231,7 @@
       <c r="AR7" s="118"/>
       <c r="AS7" s="118"/>
     </row>
-    <row r="8" spans="1:45" s="121" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" s="121" customFormat="1" ht="41.45">
       <c r="A8" s="104" t="s">
         <v>586</v>
       </c>
@@ -27324,7 +27324,7 @@
       <c r="AR8" s="118"/>
       <c r="AS8" s="118"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45">
       <c r="A11" s="126" t="s">
         <v>634</v>
       </c>
@@ -27350,17 +27350,17 @@
       <selection activeCell="S2" sqref="S2:S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5546875" customWidth="1"/>
-    <col min="5" max="5" width="42.88671875" customWidth="1"/>
-    <col min="6" max="6" width="53.88671875" customWidth="1"/>
-    <col min="7" max="7" width="43.5546875" customWidth="1"/>
-    <col min="8" max="8" width="53.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="43.5703125" customWidth="1"/>
+    <col min="8" max="8" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="138" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="138" customFormat="1" ht="55.15">
       <c r="A1" s="130" t="s">
         <v>0</v>
       </c>
@@ -27467,7 +27467,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="138" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" s="138" customFormat="1" ht="55.15">
       <c r="A2" s="130" t="s">
         <v>637</v>
       </c>
@@ -27564,7 +27564,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="3" spans="1:36" s="138" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" s="138" customFormat="1" ht="55.15">
       <c r="A3" s="130" t="s">
         <v>637</v>
       </c>
@@ -27661,7 +27661,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:36" s="138" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" s="138" customFormat="1" ht="55.15">
       <c r="A4" s="130" t="s">
         <v>637</v>
       </c>
@@ -27756,7 +27756,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="138" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" s="138" customFormat="1" ht="55.15">
       <c r="A5" s="130" t="s">
         <v>637</v>
       </c>
@@ -27851,7 +27851,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="6" spans="1:36" s="138" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" s="138" customFormat="1" ht="13.9">
       <c r="A6" s="152" t="s">
         <v>668</v>
       </c>
@@ -27860,7 +27860,7 @@
       <c r="K6" s="154"/>
       <c r="L6" s="154"/>
     </row>
-    <row r="7" spans="1:36" s="138" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" s="138" customFormat="1" ht="55.15">
       <c r="A7" s="130" t="s">
         <v>637</v>
       </c>
@@ -27956,27 +27956,27 @@
       </c>
       <c r="AJ7" s="147"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36">
       <c r="D11" s="158"/>
       <c r="E11" s="159"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36">
       <c r="D12" s="158"/>
       <c r="E12" s="159"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36">
       <c r="D13" s="158"/>
       <c r="E13" s="159"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36">
       <c r="D14" s="158"/>
       <c r="E14" s="159"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36">
       <c r="D15" s="160"/>
       <c r="E15" s="160"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36">
       <c r="D16" s="158"/>
       <c r="E16" s="158"/>
     </row>
@@ -28001,54 +28001,54 @@
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="38.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="13.15"/>
   <cols>
     <col min="1" max="1" width="8" style="252" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="252" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="252" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="38.109375" style="252"/>
-    <col min="6" max="6" width="27.6640625" style="252" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" style="252" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" style="252" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" style="252" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="252" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="252" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.140625" style="252"/>
+    <col min="6" max="6" width="27.7109375" style="252" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" style="252" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="252" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="252" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="252" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.88671875" style="252" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" style="252" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="252" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.85546875" style="252" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="252" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="252" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="252" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.109375" style="252"/>
-    <col min="17" max="17" width="18.88671875" style="252" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.109375" style="252" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.44140625" style="252" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.88671875" style="252" customWidth="1"/>
+    <col min="16" max="16" width="38.140625" style="252"/>
+    <col min="17" max="17" width="18.85546875" style="252" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="252" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.42578125" style="252" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" style="252" customWidth="1"/>
     <col min="22" max="22" width="16" style="252" customWidth="1"/>
-    <col min="23" max="23" width="11.88671875" style="252" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.88671875" style="252" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.109375" style="252" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.33203125" style="252" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.6640625" style="252" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.109375" style="252" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.5546875" style="252" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.6640625" style="252" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.6640625" style="252" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.33203125" style="252" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.5546875" style="252" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="34.109375" style="252" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.6640625" style="252" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.109375" style="252" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="252" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" style="252" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" style="252" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.28515625" style="252" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="252" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.140625" style="252" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.5703125" style="252" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.7109375" style="252" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" style="252" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.28515625" style="252" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.5703125" style="252" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="34.140625" style="252" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" style="252" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" style="252" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="26" style="252" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="27.44140625" style="252" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.5546875" style="252" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.44140625" style="252" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.5546875" style="252" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21.33203125" style="252" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="21.44140625" style="252" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27.42578125" style="252" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.5703125" style="252" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.42578125" style="252" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5703125" style="252" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21.28515625" style="252" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="21.42578125" style="252" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="21" style="252" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="38" style="252" customWidth="1"/>
-    <col min="47" max="16384" width="38.109375" style="252"/>
+    <col min="47" max="16384" width="38.140625" style="252"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="218" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" s="218" customFormat="1" ht="37.5" customHeight="1">
       <c r="A1" s="206" t="s">
         <v>0</v>
       </c>
@@ -28229,7 +28229,7 @@
       <c r="CJ1" s="217"/>
       <c r="CK1" s="217"/>
     </row>
-    <row r="2" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A2" s="206" t="s">
         <v>680</v>
       </c>
@@ -28354,7 +28354,7 @@
       <c r="BL2" s="226"/>
       <c r="BM2" s="227"/>
     </row>
-    <row r="3" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A3" s="206" t="s">
         <v>680</v>
       </c>
@@ -28477,7 +28477,7 @@
       <c r="BL3" s="226"/>
       <c r="BM3" s="227"/>
     </row>
-    <row r="4" spans="1:89" s="229" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:89" s="229" customFormat="1" ht="27.6">
       <c r="A4" s="206" t="s">
         <v>680</v>
       </c>
@@ -28626,7 +28626,7 @@
       <c r="CJ4" s="228"/>
       <c r="CK4" s="228"/>
     </row>
-    <row r="5" spans="1:89" s="229" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:89" s="229" customFormat="1" ht="27.6">
       <c r="A5" s="230" t="s">
         <v>680</v>
       </c>
@@ -28771,7 +28771,7 @@
       <c r="CJ5" s="228"/>
       <c r="CK5" s="228"/>
     </row>
-    <row r="6" spans="1:89" s="229" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:89" s="229" customFormat="1" ht="27.6">
       <c r="A6" s="206" t="s">
         <v>680</v>
       </c>
@@ -28920,7 +28920,7 @@
       <c r="CJ6" s="228"/>
       <c r="CK6" s="228"/>
     </row>
-    <row r="7" spans="1:89" s="229" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:89" s="229" customFormat="1" ht="27.6">
       <c r="A7" s="230" t="s">
         <v>680</v>
       </c>
@@ -29065,7 +29065,7 @@
       <c r="CJ7" s="228"/>
       <c r="CK7" s="228"/>
     </row>
-    <row r="8" spans="1:89" s="228" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:89" s="228" customFormat="1" ht="27.6">
       <c r="A8" s="206" t="s">
         <v>680</v>
       </c>
@@ -29190,7 +29190,7 @@
       <c r="BL8" s="226"/>
       <c r="BM8" s="227"/>
     </row>
-    <row r="9" spans="1:89" s="229" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:89" s="229" customFormat="1" ht="27.6">
       <c r="A9" s="230" t="s">
         <v>680</v>
       </c>
@@ -29335,7 +29335,7 @@
       <c r="CJ9" s="228"/>
       <c r="CK9" s="228"/>
     </row>
-    <row r="10" spans="1:89" s="229" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:89" s="229" customFormat="1" ht="41.45">
       <c r="A10" s="206" t="s">
         <v>680</v>
       </c>
@@ -29460,7 +29460,7 @@
       <c r="BL10" s="233"/>
       <c r="BM10" s="234"/>
     </row>
-    <row r="11" spans="1:89" s="229" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:89" s="229" customFormat="1" ht="41.45">
       <c r="A11" s="230" t="s">
         <v>680</v>
       </c>
@@ -29605,7 +29605,7 @@
       <c r="CJ11" s="228"/>
       <c r="CK11" s="228"/>
     </row>
-    <row r="12" spans="1:89" s="229" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:89" s="229" customFormat="1" ht="27.6">
       <c r="A12" s="206" t="s">
         <v>680</v>
       </c>
@@ -29748,7 +29748,7 @@
       <c r="CJ12" s="228"/>
       <c r="CK12" s="228"/>
     </row>
-    <row r="13" spans="1:89" s="235" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:89" s="235" customFormat="1" ht="27.6">
       <c r="A13" s="206" t="s">
         <v>680</v>
       </c>
@@ -29897,7 +29897,7 @@
       <c r="CJ13" s="228"/>
       <c r="CK13" s="228"/>
     </row>
-    <row r="14" spans="1:89" s="235" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:89" s="235" customFormat="1" ht="27.6">
       <c r="A14" s="206" t="s">
         <v>680</v>
       </c>
@@ -30044,7 +30044,7 @@
       <c r="CJ14" s="228"/>
       <c r="CK14" s="228"/>
     </row>
-    <row r="15" spans="1:89" s="228" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:89" s="228" customFormat="1" ht="27.6">
       <c r="A15" s="206" t="s">
         <v>680</v>
       </c>
@@ -30169,7 +30169,7 @@
       <c r="BL15" s="226"/>
       <c r="BM15" s="227"/>
     </row>
-    <row r="16" spans="1:89" s="228" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:89" s="228" customFormat="1" ht="27.6">
       <c r="A16" s="206" t="s">
         <v>680</v>
       </c>
@@ -30290,7 +30290,7 @@
       <c r="BL16" s="226"/>
       <c r="BM16" s="227"/>
     </row>
-    <row r="17" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A17" s="206" t="s">
         <v>680</v>
       </c>
@@ -30439,7 +30439,7 @@
       <c r="CJ17" s="229"/>
       <c r="CK17" s="229"/>
     </row>
-    <row r="18" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A18" s="206" t="s">
         <v>680</v>
       </c>
@@ -30586,7 +30586,7 @@
       <c r="CJ18" s="229"/>
       <c r="CK18" s="229"/>
     </row>
-    <row r="19" spans="1:89" s="235" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:89" s="235" customFormat="1" ht="41.45">
       <c r="A19" s="206" t="s">
         <v>680</v>
       </c>
@@ -30733,7 +30733,7 @@
       <c r="CJ19" s="228"/>
       <c r="CK19" s="228"/>
     </row>
-    <row r="20" spans="1:89" s="228" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:89" s="228" customFormat="1" ht="42.6" customHeight="1">
       <c r="A20" s="206" t="s">
         <v>680</v>
       </c>
@@ -30880,7 +30880,7 @@
       <c r="CJ20" s="229"/>
       <c r="CK20" s="229"/>
     </row>
-    <row r="21" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A21" s="206" t="s">
         <v>680</v>
       </c>
@@ -31003,7 +31003,7 @@
       <c r="BL21" s="226"/>
       <c r="BM21" s="227"/>
     </row>
-    <row r="22" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A22" s="206" t="s">
         <v>680</v>
       </c>
@@ -31126,7 +31126,7 @@
       <c r="BL22" s="226"/>
       <c r="BM22" s="227"/>
     </row>
-    <row r="23" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A23" s="206" t="s">
         <v>680</v>
       </c>
@@ -31273,7 +31273,7 @@
       <c r="CJ23" s="229"/>
       <c r="CK23" s="229"/>
     </row>
-    <row r="24" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A24" s="206" t="s">
         <v>680</v>
       </c>
@@ -31420,7 +31420,7 @@
       <c r="CJ24" s="229"/>
       <c r="CK24" s="229"/>
     </row>
-    <row r="25" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A25" s="206" t="s">
         <v>680</v>
       </c>
@@ -31567,7 +31567,7 @@
       <c r="CJ25" s="229"/>
       <c r="CK25" s="229"/>
     </row>
-    <row r="26" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A26" s="206" t="s">
         <v>680</v>
       </c>
@@ -31714,7 +31714,7 @@
       <c r="CJ26" s="229"/>
       <c r="CK26" s="229"/>
     </row>
-    <row r="27" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A27" s="206" t="s">
         <v>680</v>
       </c>
@@ -31861,7 +31861,7 @@
       <c r="CJ27" s="229"/>
       <c r="CK27" s="229"/>
     </row>
-    <row r="28" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A28" s="206" t="s">
         <v>680</v>
       </c>
@@ -32008,7 +32008,7 @@
       <c r="CJ28" s="229"/>
       <c r="CK28" s="229"/>
     </row>
-    <row r="29" spans="1:89" s="226" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:89" s="226" customFormat="1" ht="41.45">
       <c r="A29" s="206" t="s">
         <v>680</v>
       </c>
@@ -32155,7 +32155,7 @@
       <c r="CJ29" s="233"/>
       <c r="CK29" s="233"/>
     </row>
-    <row r="30" spans="1:89" s="226" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:89" s="226" customFormat="1" ht="41.45">
       <c r="A30" s="206" t="s">
         <v>680</v>
       </c>
@@ -32302,7 +32302,7 @@
       <c r="CJ30" s="233"/>
       <c r="CK30" s="233"/>
     </row>
-    <row r="31" spans="1:89" s="226" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:89" s="226" customFormat="1" ht="41.45">
       <c r="A31" s="206" t="s">
         <v>680</v>
       </c>
@@ -32449,7 +32449,7 @@
       <c r="CJ31" s="233"/>
       <c r="CK31" s="233"/>
     </row>
-    <row r="32" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A32" s="206" t="s">
         <v>680</v>
       </c>
@@ -32596,7 +32596,7 @@
       <c r="CJ32" s="229"/>
       <c r="CK32" s="229"/>
     </row>
-    <row r="33" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A33" s="206" t="s">
         <v>680</v>
       </c>
@@ -32719,7 +32719,7 @@
       <c r="BL33" s="226"/>
       <c r="BM33" s="227"/>
     </row>
-    <row r="34" spans="1:89" s="228" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:89" s="228" customFormat="1" ht="41.45">
       <c r="A34" s="206" t="s">
         <v>680</v>
       </c>
@@ -32842,7 +32842,7 @@
       <c r="BL34" s="226"/>
       <c r="BM34" s="227"/>
     </row>
-    <row r="35" spans="1:89" s="235" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:89" s="235" customFormat="1" ht="41.45">
       <c r="A35" s="206" t="s">
         <v>680</v>
       </c>
@@ -32991,7 +32991,7 @@
       <c r="CJ35" s="228"/>
       <c r="CK35" s="228"/>
     </row>
-    <row r="36" spans="1:89" s="235" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:89" s="235" customFormat="1" ht="41.45">
       <c r="A36" s="206" t="s">
         <v>680</v>
       </c>
@@ -33138,7 +33138,7 @@
       <c r="CJ36" s="228"/>
       <c r="CK36" s="228"/>
     </row>
-    <row r="37" spans="1:89" s="235" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:89" s="235" customFormat="1" ht="41.45">
       <c r="A37" s="206" t="s">
         <v>680</v>
       </c>
@@ -33287,7 +33287,7 @@
       <c r="CJ37" s="228"/>
       <c r="CK37" s="228"/>
     </row>
-    <row r="38" spans="1:89" s="235" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:89" s="235" customFormat="1" ht="41.45">
       <c r="A38" s="206" t="s">
         <v>680</v>
       </c>
@@ -33434,7 +33434,7 @@
       <c r="CJ38" s="228"/>
       <c r="CK38" s="228"/>
     </row>
-    <row r="39" spans="1:89" s="235" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:89" s="235" customFormat="1" ht="41.45">
       <c r="A39" s="206" t="s">
         <v>680</v>
       </c>
@@ -33583,7 +33583,7 @@
       <c r="CJ39" s="228"/>
       <c r="CK39" s="228"/>
     </row>
-    <row r="40" spans="1:89" s="235" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:89" s="235" customFormat="1" ht="41.45">
       <c r="A40" s="206" t="s">
         <v>680</v>
       </c>
@@ -33730,7 +33730,7 @@
       <c r="CJ40" s="228"/>
       <c r="CK40" s="228"/>
     </row>
-    <row r="41" spans="1:89" s="239" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:89" s="239" customFormat="1" ht="41.45">
       <c r="A41" s="206" t="s">
         <v>680</v>
       </c>
@@ -33877,7 +33877,7 @@
       <c r="CJ41" s="226"/>
       <c r="CK41" s="226"/>
     </row>
-    <row r="42" spans="1:89" s="239" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:89" s="239" customFormat="1" ht="41.45">
       <c r="A42" s="206" t="s">
         <v>680</v>
       </c>
@@ -34024,7 +34024,7 @@
       <c r="CJ42" s="226"/>
       <c r="CK42" s="226"/>
     </row>
-    <row r="43" spans="1:89" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:89" ht="41.45">
       <c r="A43" s="206" t="s">
         <v>680</v>
       </c>
@@ -34127,7 +34127,7 @@
       <c r="AR43" s="293"/>
       <c r="AS43" s="293"/>
     </row>
-    <row r="44" spans="1:89" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:89" ht="41.45">
       <c r="A44" s="206" t="s">
         <v>680</v>
       </c>
@@ -34233,12 +34233,16 @@
   </sheetData>
   <autoFilter ref="A1:CK1" xr:uid="{81481555-CC8D-496A-8B62-D9F1569CF07D}"/>
   <mergeCells count="28">
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="Q16:R16"/>
@@ -34251,16 +34255,12 @@
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q11:R11"/>
   </mergeCells>
   <conditionalFormatting sqref="P1:R1">
     <cfRule type="expression" dxfId="28" priority="1" stopIfTrue="1">

</xml_diff>

<commit_message>
Añadido columna silencio autorizaciones. Arreglo tabla permisos(no cargaba pagina EX01).
</commit_message>
<xml_diff>
--- a/01-carga-excel/sqlite/docs/excel-cod.xlsx
+++ b/01-carga-excel/sqlite/docs/excel-cod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E08DCAC3-7FD5-4D7E-9412-48724040E25B}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{484BF7F5-D8BB-46FC-95B0-2C8099126380}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="10" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="10" activeTab="14" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -6432,8 +6432,8 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="D26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8509,7 +8509,7 @@
   </sheetPr>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -10715,10 +10715,10 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" customWidth="1"/>
@@ -10731,7 +10731,7 @@
     <col min="35" max="35" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="41.45">
+    <row r="1" spans="1:36" ht="44.25">
       <c r="A1" s="275" t="s">
         <v>953</v>
       </c>
@@ -11137,8 +11137,8 @@
   </sheetPr>
   <dimension ref="A1:CK7"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.45"/>
@@ -14574,8 +14574,8 @@
   </sheetPr>
   <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView topLeftCell="Q20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="14.45"/>
@@ -17287,8 +17287,8 @@
   </sheetPr>
   <dimension ref="A1:CK5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -17855,8 +17855,8 @@
   </sheetPr>
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -18003,7 +18003,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="41.45">
+    <row r="2" spans="1:45" ht="27">
       <c r="A2" s="1" t="s">
         <v>194</v>
       </c>
@@ -18364,8 +18364,8 @@
   </sheetPr>
   <dimension ref="A1:CK15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -20602,8 +20602,8 @@
   </sheetPr>
   <dimension ref="A1:CK30"/>
   <sheetViews>
-    <sheetView topLeftCell="I21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L23" sqref="K23:L23"/>
+    <sheetView topLeftCell="E25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16:T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.15"/>
@@ -22707,7 +22707,7 @@
       <c r="BL15" s="226"/>
       <c r="BM15" s="227"/>
     </row>
-    <row r="16" spans="1:89" s="228" customFormat="1" ht="110.45">
+    <row r="16" spans="1:89" s="228" customFormat="1" ht="94.5">
       <c r="A16" s="224" t="s">
         <v>318</v>
       </c>
@@ -25853,7 +25853,7 @@
   </sheetPr>
   <dimension ref="A1:CI7"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -26547,8 +26547,8 @@
   </sheetPr>
   <dimension ref="A1:AS11"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -27346,7 +27346,7 @@
   </sheetPr>
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="S2" sqref="S2:S7"/>
     </sheetView>
   </sheetViews>
@@ -27997,8 +27997,8 @@
   </sheetPr>
   <dimension ref="A1:CK44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="13.15"/>

</xml_diff>

<commit_message>
Eliminacion columna duracion maxima (M, EX19)
</commit_message>
<xml_diff>
--- a/01-carga-excel/sqlite/docs/excel-cod.xlsx
+++ b/01-carga-excel/sqlite/docs/excel-cod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{484BF7F5-D8BB-46FC-95B0-2C8099126380}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE495DEA-9E75-4A44-844E-E0343227F545}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="10" activeTab="14" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="10" activeTab="10" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -6432,8 +6432,8 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="D26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+    <sheetView topLeftCell="D18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8366,7 +8366,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="55.15">
+    <row r="31" spans="1:23" ht="53.25">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -17288,7 +17288,7 @@
   <dimension ref="A1:CK5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>